<commit_message>
Added SEASON to PV and DH solar heating and constrained DH solar heating per TS
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Time_Slices.xlsx
+++ b/SuppXLS/Scen_Time_Slices.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="15">
   <si>
     <t>Attribute</t>
   </si>
@@ -68,6 +68,9 @@
   <si>
     <t>ERWIN1E</t>
   </si>
+  <si>
+    <t>EHSOLHT1E</t>
+  </si>
 </sst>
 </file>
 
@@ -79,7 +82,7 @@
     <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0;\-\ #,##0;_-\ &quot;- &quot;"/>
     <numFmt numFmtId="166" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-"/>
-    <numFmt numFmtId="168" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="33" x14ac:knownFonts="1">
     <font>
@@ -874,7 +877,7 @@
     <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4342,10 +4345,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B4:E21"/>
+  <dimension ref="B4:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5107,6 +5110,62 @@
         <v>13</v>
       </c>
     </row>
+    <row r="22" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.10829415070669778</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.12417253524194671</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="6">
+        <v>4.2282889155662889E-2</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="6">
+        <v>3.0775520587982483E-2</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>